<commit_message>
Update DAD Data Dictionary 2019.xlsx
</commit_message>
<xml_diff>
--- a/DAD Data Dictionary 2019.xlsx
+++ b/DAD Data Dictionary 2019.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yun.yao\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yun.yao\Documents\Dashboard 2019\DAD-2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8811" uniqueCount="1708">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8811" uniqueCount="1707">
   <si>
     <t>Label</t>
   </si>
@@ -5119,18 +5119,12 @@
     <t>For ACCCESS, and Alt ACCESS</t>
   </si>
   <si>
-    <t>00-600</t>
-  </si>
-  <si>
     <t>SS_Speak</t>
   </si>
   <si>
     <t>Scaled Score, Speaking</t>
   </si>
   <si>
-    <t>0-600</t>
-  </si>
-  <si>
     <t>For ACCCESS and Alt ACCESS</t>
   </si>
   <si>
@@ -5168,6 +5162,9 @@
   </si>
   <si>
     <t>CBT_Write</t>
+  </si>
+  <si>
+    <t>0-1000</t>
   </si>
 </sst>
 </file>
@@ -5704,8 +5701,8 @@
   <dimension ref="A1:Q1509"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N49" sqref="N49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6324,7 +6321,7 @@
         <v>1</v>
       </c>
       <c r="Q13" s="16" t="s">
-        <v>1702</v>
+        <v>1700</v>
       </c>
     </row>
     <row r="14" spans="1:17" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -6371,7 +6368,7 @@
         <v>1</v>
       </c>
       <c r="Q14" s="16" t="s">
-        <v>1702</v>
+        <v>1700</v>
       </c>
     </row>
     <row r="15" spans="1:17" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -6418,7 +6415,7 @@
         <v>1</v>
       </c>
       <c r="Q15" s="16" t="s">
-        <v>1702</v>
+        <v>1700</v>
       </c>
     </row>
     <row r="16" spans="1:17" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -6465,7 +6462,7 @@
         <v>1</v>
       </c>
       <c r="Q16" s="16" t="s">
-        <v>1702</v>
+        <v>1700</v>
       </c>
     </row>
     <row r="17" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -6662,7 +6659,7 @@
         <v>20</v>
       </c>
       <c r="E21" s="38" t="s">
-        <v>1704</v>
+        <v>1702</v>
       </c>
       <c r="F21" s="16" t="s">
         <v>182</v>
@@ -6694,7 +6691,7 @@
         <v>0</v>
       </c>
       <c r="Q21" s="16" t="s">
-        <v>1702</v>
+        <v>1700</v>
       </c>
     </row>
     <row r="22" spans="1:17" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -6709,7 +6706,7 @@
         <v>21</v>
       </c>
       <c r="E22" s="38" t="s">
-        <v>1705</v>
+        <v>1703</v>
       </c>
       <c r="F22" s="16" t="s">
         <v>182</v>
@@ -6741,7 +6738,7 @@
         <v>0</v>
       </c>
       <c r="Q22" s="16" t="s">
-        <v>1702</v>
+        <v>1700</v>
       </c>
     </row>
     <row r="23" spans="1:17" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -6756,7 +6753,7 @@
         <v>22</v>
       </c>
       <c r="E23" s="38" t="s">
-        <v>1706</v>
+        <v>1704</v>
       </c>
       <c r="F23" s="16" t="s">
         <v>182</v>
@@ -6788,7 +6785,7 @@
         <v>0</v>
       </c>
       <c r="Q23" s="16" t="s">
-        <v>1702</v>
+        <v>1700</v>
       </c>
     </row>
     <row r="24" spans="1:17" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -6803,7 +6800,7 @@
         <v>23</v>
       </c>
       <c r="E24" s="38" t="s">
-        <v>1707</v>
+        <v>1705</v>
       </c>
       <c r="F24" s="16" t="s">
         <v>182</v>
@@ -6835,7 +6832,7 @@
         <v>0</v>
       </c>
       <c r="Q24" s="16" t="s">
-        <v>1702</v>
+        <v>1700</v>
       </c>
     </row>
     <row r="25" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -7109,7 +7106,7 @@
         <v>1</v>
       </c>
       <c r="Q30" s="16" t="s">
-        <v>1702</v>
+        <v>1700</v>
       </c>
     </row>
     <row r="31" spans="1:17" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -7156,7 +7153,7 @@
         <v>1</v>
       </c>
       <c r="Q31" s="16" t="s">
-        <v>1702</v>
+        <v>1700</v>
       </c>
     </row>
     <row r="32" spans="1:17" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -7203,7 +7200,7 @@
         <v>1</v>
       </c>
       <c r="Q32" s="16" t="s">
-        <v>1702</v>
+        <v>1700</v>
       </c>
     </row>
     <row r="33" spans="1:17" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -7250,7 +7247,7 @@
         <v>1</v>
       </c>
       <c r="Q33" s="16" t="s">
-        <v>1702</v>
+        <v>1700</v>
       </c>
     </row>
     <row r="34" spans="1:17" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -7297,7 +7294,7 @@
         <v>1</v>
       </c>
       <c r="Q34" s="16" t="s">
-        <v>1702</v>
+        <v>1700</v>
       </c>
     </row>
     <row r="35" spans="1:17" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -7344,7 +7341,7 @@
         <v>1</v>
       </c>
       <c r="Q35" s="16" t="s">
-        <v>1702</v>
+        <v>1700</v>
       </c>
     </row>
     <row r="36" spans="1:17" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -7391,7 +7388,7 @@
         <v>1</v>
       </c>
       <c r="Q36" s="16" t="s">
-        <v>1702</v>
+        <v>1700</v>
       </c>
     </row>
     <row r="37" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -7566,14 +7563,14 @@
       </c>
       <c r="M40" s="16"/>
       <c r="N40" s="19" t="s">
-        <v>1691</v>
+        <v>1706</v>
       </c>
       <c r="O40" s="16"/>
       <c r="P40" s="16">
         <v>1</v>
       </c>
       <c r="Q40" s="16" t="s">
-        <v>1695</v>
+        <v>1693</v>
       </c>
     </row>
     <row r="41" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -7613,7 +7610,7 @@
       </c>
       <c r="M41" s="16"/>
       <c r="N41" s="19" t="s">
-        <v>1691</v>
+        <v>1706</v>
       </c>
       <c r="O41" s="16"/>
       <c r="P41" s="16">
@@ -7635,10 +7632,10 @@
         <v>41</v>
       </c>
       <c r="E42" s="38" t="s">
+        <v>1691</v>
+      </c>
+      <c r="F42" s="16" t="s">
         <v>1692</v>
-      </c>
-      <c r="F42" s="16" t="s">
-        <v>1693</v>
       </c>
       <c r="G42" s="16" t="s">
         <v>15</v>
@@ -7660,7 +7657,7 @@
       </c>
       <c r="M42" s="16"/>
       <c r="N42" s="19" t="s">
-        <v>1694</v>
+        <v>1706</v>
       </c>
       <c r="O42" s="16"/>
       <c r="P42" s="16">
@@ -7707,7 +7704,7 @@
       </c>
       <c r="M43" s="16"/>
       <c r="N43" s="19" t="s">
-        <v>1694</v>
+        <v>1706</v>
       </c>
       <c r="O43" s="16"/>
       <c r="P43" s="16">
@@ -7729,10 +7726,10 @@
         <v>43</v>
       </c>
       <c r="E44" s="38" t="s">
+        <v>1694</v>
+      </c>
+      <c r="F44" s="16" t="s">
         <v>1696</v>
-      </c>
-      <c r="F44" s="16" t="s">
-        <v>1698</v>
       </c>
       <c r="G44" s="16" t="s">
         <v>15</v>
@@ -7754,14 +7751,14 @@
       </c>
       <c r="M44" s="16"/>
       <c r="N44" s="19" t="s">
-        <v>1694</v>
+        <v>1706</v>
       </c>
       <c r="O44" s="16"/>
       <c r="P44" s="16">
         <v>1</v>
       </c>
       <c r="Q44" s="16" t="s">
-        <v>1703</v>
+        <v>1701</v>
       </c>
     </row>
     <row r="45" spans="1:17" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -7776,10 +7773,10 @@
         <v>44</v>
       </c>
       <c r="E45" s="38" t="s">
+        <v>1695</v>
+      </c>
+      <c r="F45" s="16" t="s">
         <v>1697</v>
-      </c>
-      <c r="F45" s="16" t="s">
-        <v>1699</v>
       </c>
       <c r="G45" s="16" t="s">
         <v>15</v>
@@ -7801,14 +7798,14 @@
       </c>
       <c r="M45" s="16"/>
       <c r="N45" s="19" t="s">
-        <v>1694</v>
+        <v>1706</v>
       </c>
       <c r="O45" s="16"/>
       <c r="P45" s="16">
         <v>1</v>
       </c>
       <c r="Q45" s="16" t="s">
-        <v>1703</v>
+        <v>1701</v>
       </c>
     </row>
     <row r="46" spans="1:17" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -7823,10 +7820,10 @@
         <v>45</v>
       </c>
       <c r="E46" s="38" t="s">
-        <v>1701</v>
+        <v>1699</v>
       </c>
       <c r="F46" s="16" t="s">
-        <v>1700</v>
+        <v>1698</v>
       </c>
       <c r="G46" s="16" t="s">
         <v>15</v>
@@ -7848,14 +7845,14 @@
       </c>
       <c r="M46" s="16"/>
       <c r="N46" s="19" t="s">
-        <v>1694</v>
+        <v>1706</v>
       </c>
       <c r="O46" s="16"/>
       <c r="P46" s="16">
         <v>1</v>
       </c>
       <c r="Q46" s="16" t="s">
-        <v>1703</v>
+        <v>1701</v>
       </c>
     </row>
     <row r="47" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>